<commit_message>
Final Patch Update before release
</commit_message>
<xml_diff>
--- a/data/Map001.xlsx
+++ b/data/Map001.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="269">
   <si>
     <t>&lt;Darkness:20&gt;</t>
   </si>
@@ -716,6 +716,9 @@
   </si>
   <si>
     <t>ライム</t>
+  </si>
+  <si>
+    <t>Lime</t>
   </si>
   <si>
     <t>\n&lt;\n[3]&gt;はい♥
@@ -1987,6 +1990,9 @@
       <c r="C116" t="s">
         <v>115</v>
       </c>
+      <c r="D116" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="117" spans="1:4">
       <c r="A117" t="s">
@@ -2135,6 +2141,9 @@
       <c r="C145" t="s">
         <v>145</v>
       </c>
+      <c r="D145" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="146" spans="1:4">
       <c r="A146" t="s">
@@ -2313,415 +2322,418 @@
       <c r="A174" t="s">
         <v>185</v>
       </c>
+      <c r="D174" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="175" spans="1:4">
       <c r="A175" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="176" spans="1:4">
       <c r="A176" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="177" spans="1:4">
       <c r="A177" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="178" spans="1:4">
       <c r="A178" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="179" spans="1:4">
       <c r="A179" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="180" spans="1:4">
       <c r="A180" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="181" spans="1:4">
       <c r="A181" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="182" spans="1:4">
       <c r="A182" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="183" spans="1:4">
       <c r="A183" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="184" spans="1:4">
       <c r="A184" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="185" spans="1:4">
       <c r="A185" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="186" spans="1:4">
       <c r="A186" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="187" spans="1:4">
       <c r="A187" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="188" spans="1:4">
       <c r="A188" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="189" spans="1:4">
       <c r="A189" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="190" spans="1:4">
       <c r="A190" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="191" spans="1:4">
       <c r="A191" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="192" spans="1:4">
       <c r="A192" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="193" spans="1:4">
       <c r="A193" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="194" spans="1:4">
       <c r="A194" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="195" spans="1:4">
       <c r="A195" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="196" spans="1:4">
       <c r="A196" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="197" spans="1:4">
       <c r="A197" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="198" spans="1:4">
       <c r="A198" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="199" spans="1:4">
       <c r="A199" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="200" spans="1:4">
       <c r="A200" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="201" spans="1:4">
       <c r="A201" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="202" spans="1:4">
       <c r="A202" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="203" spans="1:4">
       <c r="A203" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="204" spans="1:4">
       <c r="A204" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="205" spans="1:4">
       <c r="A205" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="206" spans="1:4">
       <c r="A206" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="207" spans="1:4">
       <c r="A207" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="208" spans="1:4">
       <c r="A208" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="209" spans="1:4">
       <c r="A209" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="210" spans="1:4">
       <c r="A210" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="211" spans="1:4">
       <c r="A211" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="212" spans="1:4">
       <c r="A212" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="213" spans="1:4">
       <c r="A213" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="214" spans="1:4">
       <c r="A214" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="215" spans="1:4">
       <c r="A215" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="216" spans="1:4">
       <c r="A216" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="217" spans="1:4">
       <c r="A217" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="218" spans="1:4">
       <c r="A218" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="219" spans="1:4">
       <c r="A219" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="220" spans="1:4">
       <c r="A220" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="221" spans="1:4">
       <c r="A221" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="222" spans="1:4">
       <c r="A222" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="223" spans="1:4">
       <c r="A223" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="224" spans="1:4">
       <c r="A224" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="225" spans="1:4">
       <c r="A225" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="226" spans="1:4">
       <c r="A226" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="227" spans="1:4">
       <c r="A227" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="228" spans="1:4">
       <c r="A228" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="229" spans="1:4">
       <c r="A229" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="230" spans="1:4">
       <c r="A230" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="231" spans="1:4">
       <c r="A231" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="232" spans="1:4">
       <c r="A232" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="233" spans="1:4">
       <c r="A233" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="234" spans="1:4">
       <c r="A234" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="235" spans="1:4">
       <c r="A235" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="236" spans="1:4">
       <c r="A236" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="237" spans="1:4">
       <c r="A237" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="238" spans="1:4">
       <c r="A238" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="239" spans="1:4">
       <c r="A239" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="240" spans="1:4">
       <c r="A240" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="241" spans="1:4">
       <c r="A241" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="242" spans="1:4">
       <c r="A242" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="243" spans="1:4">
       <c r="A243" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="244" spans="1:4">
       <c r="A244" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="245" spans="1:4">
       <c r="A245" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="246" spans="1:4">
       <c r="A246" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="247" spans="1:4">
       <c r="A247" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="248" spans="1:4">
       <c r="A248" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="249" spans="1:4">
       <c r="A249" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="250" spans="1:4">
       <c r="A250" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="251" spans="1:4">
       <c r="A251" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="252" spans="1:4">
       <c r="A252" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="253" spans="1:4">
       <c r="A253" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="254" spans="1:4">
       <c r="A254" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="255" spans="1:4">
       <c r="A255" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="256" spans="1:4">
       <c r="A256" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>

</xml_diff>